<commit_message>
testing full row 1
</commit_message>
<xml_diff>
--- a/excel/Source Spreadsheet Updated.xlsx
+++ b/excel/Source Spreadsheet Updated.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28318"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0C29DC2-32DD-4003-94FB-13DCBF47E94A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CBF471E0-425E-4E50-A1F7-62CCF6EEB8BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,9 +31,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>TITLE TO SKIP</t>
+  </si>
+  <si>
+    <t>placeholder</t>
   </si>
   <si>
     <t>ID</t>
@@ -169,7 +172,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -186,10 +189,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,43 +411,55 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:G2"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" ht="12.75">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="12.75">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -455,7 +467,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" s="3" t="b">
         <v>0</v>
@@ -467,7 +479,7 @@
         <v>87.864999999999995</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G3" s="3">
         <v>3</v>
@@ -478,7 +490,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" s="3" t="b">
         <v>1</v>
@@ -490,7 +502,7 @@
         <v>90.531999999999996</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G4" s="3">
         <v>6</v>
@@ -501,7 +513,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="3" t="b">
         <v>1</v>
@@ -513,7 +525,7 @@
         <v>74.034999999999997</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G5" s="3">
         <v>9</v>
@@ -524,7 +536,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" s="3" t="b">
         <v>0</v>
@@ -536,7 +548,7 @@
         <v>79.344999999999999</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G6" s="3">
         <v>1</v>
@@ -547,7 +559,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C7" s="4" t="b">
         <v>1</v>
@@ -559,7 +571,7 @@
         <v>35.542999999999999</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G7" s="4">
         <v>2</v>
@@ -570,7 +582,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8" s="4" t="b">
         <v>0</v>
@@ -582,7 +594,7 @@
         <v>65.733999999999995</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G8" s="4">
         <v>7</v>
@@ -593,7 +605,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C9" s="4" t="b">
         <v>0</v>
@@ -605,7 +617,7 @@
         <v>23.634</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G9" s="4">
         <v>8</v>
@@ -636,9 +648,6 @@
       <c r="F12" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
-  </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
 </worksheet>
 </file>
</xml_diff>